<commit_message>
Added realtime chart update example from clement
</commit_message>
<xml_diff>
--- a/Data/BIRT Engineer Examples.xlsx
+++ b/Data/BIRT Engineer Examples.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>#experts-BIRT email sent 3/3/2014 1:48 PM</t>
+  </si>
+  <si>
+    <t>Chart with  realtime data</t>
+  </si>
+  <si>
+    <t>Displays a chart that continuously refreshes with updated realtime date.  This example uses random data generated in the Edit Chart &gt; Script &gt;Interactivity &gt; Chart Area &gt; Load.</t>
+  </si>
+  <si>
+    <t>#experts-BIRT email sent 27/23/2014 2:46 PM Eastern</t>
+  </si>
+  <si>
+    <t>Report Designs/Charts/HTML5 Charts - Dynamic Updating Highchart__cwong.rptdesign</t>
   </si>
 </sst>
 </file>
@@ -648,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,6 +1071,26 @@
       </c>
       <c r="F20" t="s">
         <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Chart Tooltip control example, dynamic map drilldown example, fastFilter example, and change report name in titlebar example
</commit_message>
<xml_diff>
--- a/Data/BIRT Engineer Examples.xlsx
+++ b/Data/BIRT Engineer Examples.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
   <si>
     <t>Description</t>
   </si>
@@ -315,10 +315,64 @@
     <t>Displays a chart that continuously refreshes with updated realtime date.  This example uses random data generated in the Edit Chart &gt; Script &gt;Interactivity &gt; Chart Area &gt; Load.</t>
   </si>
   <si>
-    <t>#experts-BIRT email sent 27/23/2014 2:46 PM Eastern</t>
-  </si>
-  <si>
     <t>Report Designs/Charts/HTML5 Charts - Dynamic Updating Highchart__cwong.rptdesign</t>
+  </si>
+  <si>
+    <t>Filter and Search from Header</t>
+  </si>
+  <si>
+    <t>Filter a table based on a search for a string either within the entire table, or within a single column.  Script in onContentUpdate and BeforeFactory</t>
+  </si>
+  <si>
+    <t>Bill Clark</t>
+  </si>
+  <si>
+    <t>#experts-BIRT email sent 7/23/2014 2:46 PM Eastern</t>
+  </si>
+  <si>
+    <t>#experts-BIRT email sent 7/29/2014</t>
+  </si>
+  <si>
+    <t>Report Designs/JSAPI/FastFilterDetailDemo.rptdesign</t>
+  </si>
+  <si>
+    <t>Changes the name that is displayed in the title bar through scripting in OnContentUpdate</t>
+  </si>
+  <si>
+    <t>Rob Murphy</t>
+  </si>
+  <si>
+    <t>#experts-BIRT email sent 7/15/2014</t>
+  </si>
+  <si>
+    <t>Report Designs/Scripting/ChangeReportNameInTitleBar.rptdesign</t>
+  </si>
+  <si>
+    <t>Change report  name in title bar</t>
+  </si>
+  <si>
+    <t>Report Designs/Charts/ChartTooltip__cwong.rptdesign</t>
+  </si>
+  <si>
+    <t>#experts-BIRT email sent 6/30/2014</t>
+  </si>
+  <si>
+    <t>Control the size and placement of tooltip</t>
+  </si>
+  <si>
+    <t>Uses scripting to control the size and placement of the tooltip on an HTML5 chart.  The scripting is in the script tab on the chart.</t>
+  </si>
+  <si>
+    <t>Report Designs/Maps/US Populations by State Map.rptdesign</t>
+  </si>
+  <si>
+    <t>Glenn Hess, Pierre Tessier</t>
+  </si>
+  <si>
+    <t>Drilldown to any state map</t>
+  </si>
+  <si>
+    <t>This shows how to drill down from a map of the US to a map of any state.  The DynamicStateMapByCounty report design takes a state short name as a parameter.  In the beforeFactory script, the report design's map property for the XMLRepresentation is updated based on the parameter value.</t>
   </si>
 </sst>
 </file>
@@ -660,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,10 +1141,87 @@
         <v>5</v>
       </c>
       <c r="E21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" t="s">
         <v>99</v>
       </c>
-      <c r="F21" t="s">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>